<commit_message>
File Calcolo ore giusto
</commit_message>
<xml_diff>
--- a/CalcoloOre.xlsx
+++ b/CalcoloOre.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">Data</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">Ore</t>
   </si>
   <si>
+    <t xml:space="preserve">Commenti</t>
+  </si>
+  <si>
     <t xml:space="preserve">18/06 – 25/06 </t>
   </si>
   <si>
@@ -43,6 +46,9 @@
     <t xml:space="preserve">Test di comunicazione, malfunzionamento di GPIO poi risolto</t>
   </si>
   <si>
+    <t xml:space="preserve">Questo errore e’ stato un grande time sink</t>
+  </si>
+  <si>
     <t xml:space="preserve">04/07 – 11/07</t>
   </si>
   <si>
@@ -70,22 +76,43 @@
     <t xml:space="preserve">09/08 – 14/08</t>
   </si>
   <si>
-    <t xml:space="preserve">Studio su zabbix e simulazione, inizialmente possibilita’ di usare zax, passato poi ad oggetti trapper</t>
+    <t xml:space="preserve">Studio su zabbix e simulazione, inizialmente possibilita’ di usare zax</t>
   </si>
   <si>
     <t xml:space="preserve">23/08 – 30/08</t>
   </si>
   <si>
+    <t xml:space="preserve">Studio di come Zax funzionerebbe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potevo ottimizzare meglio il tempo, altro grande time sink per una priorita’ sbagliata.</t>
+  </si>
+  <si>
     <t xml:space="preserve">04/09 – 07/09</t>
   </si>
   <si>
+    <t xml:space="preserve">Passaggio ad oggetti trap</t>
+  </si>
+  <si>
     <t xml:space="preserve">10/09 – 19/09</t>
   </si>
   <si>
+    <t xml:space="preserve">Lavoro su script di export + prova a script completo di configurazione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avendo studiato questi meglio il completamento di questa parte e’ stato molto piu’ veloce</t>
+  </si>
+  <si>
     <t xml:space="preserve">19/09 – 26/09</t>
   </si>
   <si>
+    <t xml:space="preserve">Integrazione con file sender</t>
+  </si>
+  <si>
     <t xml:space="preserve">27/09 – 1/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultimi test</t>
   </si>
   <si>
     <t xml:space="preserve">Ore totali:</t>
@@ -103,6 +130,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -184,16 +212,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="140.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="81.28"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -206,13 +234,16 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>40</v>
@@ -220,21 +251,24 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>25</v>
@@ -242,21 +276,21 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>20</v>
@@ -264,10 +298,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>20</v>
@@ -275,62 +309,83 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>19</v>
+        <v>24</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>1</v>
+        <v>70</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>30</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">SUM(C2:C13)</f>
-        <v>171</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>